<commit_message>
counter free console ds
</commit_message>
<xml_diff>
--- a/grossry.xlsx
+++ b/grossry.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>rice</t>
   </si>
@@ -51,13 +51,23 @@
   <si>
     <t>avishekOnline</t>
   </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>mouth Fresh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -104,9 +114,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -464,10 +475,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -475,9 +486,11 @@
     <col min="1" max="1" width="23.1796875" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -485,7 +498,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -494,6 +507,24 @@
       </c>
       <c r="C2" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>18800</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>11200</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>